<commit_message>
Excel files for 2017 update.
</commit_message>
<xml_diff>
--- a/excel/rubrieken.xlsx
+++ b/excel/rubrieken.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="123820"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\RoelKerst2011\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Muzieklijstjes2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="597">
   <si>
     <t>Code</t>
   </si>
@@ -1345,12 +1345,480 @@
   </si>
   <si>
     <t>Domburg Draait Door</t>
+  </si>
+  <si>
+    <t>VvdM</t>
+  </si>
+  <si>
+    <t>Vinyl van de Maand</t>
+  </si>
+  <si>
+    <t>HTB132</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Aretha Franklin</t>
+  </si>
+  <si>
+    <t>HTB133</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy No wave</t>
+  </si>
+  <si>
+    <t>HTB134</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy David Bowie</t>
+  </si>
+  <si>
+    <t>HTB135</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Fleetwood mac</t>
+  </si>
+  <si>
+    <t>HTB136</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Roxy music</t>
+  </si>
+  <si>
+    <t>HTB137</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Jerry Lee Lewis</t>
+  </si>
+  <si>
+    <t>HTB138</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Paul Simon</t>
+  </si>
+  <si>
+    <t>HTB139</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy The Clash and Solo</t>
+  </si>
+  <si>
+    <t>HTB140</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Black sabbath</t>
+  </si>
+  <si>
+    <t>HTB141</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Roy Harper</t>
+  </si>
+  <si>
+    <t>HTB142</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Charles Mingus</t>
+  </si>
+  <si>
+    <t>HTB143</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Lee 'Scratch' Perry</t>
+  </si>
+  <si>
+    <t>HTB144</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Sandy Denny</t>
+  </si>
+  <si>
+    <t>HTB145</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Nina Simone</t>
+  </si>
+  <si>
+    <t>HTB146</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Hüsker dü and solo</t>
+  </si>
+  <si>
+    <t>HTB147</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Will Oldham etc.</t>
+  </si>
+  <si>
+    <t>HTB148</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy the Flaming lips</t>
+  </si>
+  <si>
+    <t>HTB149</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Marvin Gaye</t>
+  </si>
+  <si>
+    <t>HTB150</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Shoegaze</t>
+  </si>
+  <si>
+    <t>HTB151</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Yes</t>
+  </si>
+  <si>
+    <t>HTB152</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Iggy Pop</t>
+  </si>
+  <si>
+    <t>HTB153</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Elton John</t>
+  </si>
+  <si>
+    <t>HTB154</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Duke Ellington</t>
+  </si>
+  <si>
+    <t>HTB155</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Blur</t>
+  </si>
+  <si>
+    <t>HTB156</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Marc Bolan</t>
+  </si>
+  <si>
+    <t>HTB157</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Wire</t>
+  </si>
+  <si>
+    <t>HTB158</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Pink floyd</t>
+  </si>
+  <si>
+    <t>HTB159</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Radiohead</t>
+  </si>
+  <si>
+    <t>HTB160</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy The Who</t>
+  </si>
+  <si>
+    <t>HTB161</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Van Morrison</t>
+  </si>
+  <si>
+    <t>HTB162</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Neil Young</t>
+  </si>
+  <si>
+    <t>HTB163</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Randy Newman</t>
+  </si>
+  <si>
+    <t>HTB164</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Eric Clapton</t>
+  </si>
+  <si>
+    <t>HTB165</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy R.E.M.</t>
+  </si>
+  <si>
+    <t>HTB166</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy John Lydon</t>
+  </si>
+  <si>
+    <t>HTB167</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Dylan in the 60s</t>
+  </si>
+  <si>
+    <t>HTB168</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Sun Ra</t>
+  </si>
+  <si>
+    <t>HTB169</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Bruce Springsteen</t>
+  </si>
+  <si>
+    <t>HTB170</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Rare psych vinyl</t>
+  </si>
+  <si>
+    <t>HTB171</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy King Tubby</t>
+  </si>
+  <si>
+    <t>HTB172</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Dolly Parton</t>
+  </si>
+  <si>
+    <t>HTB173</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Faces and solo</t>
+  </si>
+  <si>
+    <t>HTB174</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Rory Gallagher</t>
+  </si>
+  <si>
+    <t>HTB175</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy John Coltrane</t>
+  </si>
+  <si>
+    <t>HTB176</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Manic street preachers</t>
+  </si>
+  <si>
+    <t>HTB177</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Santana</t>
+  </si>
+  <si>
+    <t>HTB178</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Ennio Morricone</t>
+  </si>
+  <si>
+    <t>HTB179</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Townes van Zandt</t>
+  </si>
+  <si>
+    <t>HTB180</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Sly Stone</t>
+  </si>
+  <si>
+    <t>HTB181</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Little feat</t>
+  </si>
+  <si>
+    <t>HTB182</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy B.B. King</t>
+  </si>
+  <si>
+    <t>HTB183</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Depeche mode</t>
+  </si>
+  <si>
+    <t>HTB184</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Cocteau twins</t>
+  </si>
+  <si>
+    <t>HTB185</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Dischord records</t>
+  </si>
+  <si>
+    <t>HTB186</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Jack White</t>
+  </si>
+  <si>
+    <t>HTB187</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Ace</t>
+  </si>
+  <si>
+    <t>HTB188</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Jeff Tweedy</t>
+  </si>
+  <si>
+    <t>HTB189</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Bee gees</t>
+  </si>
+  <si>
+    <t>HTB190</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Magma</t>
+  </si>
+  <si>
+    <t>HTB191</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Earth, wind &amp; fire</t>
+  </si>
+  <si>
+    <t>HTB192</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Pet shop boys</t>
+  </si>
+  <si>
+    <t>HTB193</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy John Cale</t>
+  </si>
+  <si>
+    <t>HTB194</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy PJ Harvey</t>
+  </si>
+  <si>
+    <t>HTB195</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Aphex twin</t>
+  </si>
+  <si>
+    <t>HTB196</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Alice Cooper</t>
+  </si>
+  <si>
+    <t>HTB197</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Isaac Hayes</t>
+  </si>
+  <si>
+    <t>HTB198</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Arthur Russell</t>
+  </si>
+  <si>
+    <t>HTB199</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Curtis Mayfield</t>
+  </si>
+  <si>
+    <t>HTB200</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Bill Evans</t>
+  </si>
+  <si>
+    <t>HTB201</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Bill Callahan/Smog</t>
+  </si>
+  <si>
+    <t>VPOTM</t>
+  </si>
+  <si>
+    <t>Vinyl package of the Month</t>
+  </si>
+  <si>
+    <t>HTB202</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Shirley Collins</t>
+  </si>
+  <si>
+    <t>HTB203</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Loudon Wainwright III</t>
+  </si>
+  <si>
+    <t>HTB204</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Popol vuh</t>
+  </si>
+  <si>
+    <t>HTB205</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Warren Zevon</t>
+  </si>
+  <si>
+    <t>HTB206</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Al Green</t>
+  </si>
+  <si>
+    <t>HTB207</t>
+  </si>
+  <si>
+    <t>Mojo - How to buy Richard Thompson</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1703,13 +2171,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D225"/>
+  <dimension ref="A1:E303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B238" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="B256" sqref="B256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,9 +2186,10 @@
     <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1733,265 +2202,247 @@
       <c r="D1" s="1" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>203</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B11" t="s">
         <v>210</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>381</v>
-      </c>
-      <c r="B7" t="s">
-        <v>382</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>439</v>
-      </c>
-      <c r="B10" t="s">
-        <v>440</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>416</v>
-      </c>
-      <c r="B11" t="s">
-        <v>431</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="D11">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>437</v>
+        <v>211</v>
       </c>
       <c r="B12" t="s">
-        <v>438</v>
+        <v>210</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>381</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>382</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>204</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>205</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>418</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>433</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>2015</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>420</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>435</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17">
-        <v>2015</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>417</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>432</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
-      <c r="D18">
-        <v>2015</v>
-      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>419</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>434</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19">
-        <v>2015</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>411</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>412</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>415</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>428</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21">
-        <v>2015</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>413</v>
+        <v>439</v>
       </c>
       <c r="B22" t="s">
-        <v>426</v>
+        <v>440</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
       </c>
-      <c r="D22">
-        <v>2015</v>
-      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B23" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -2002,24 +2453,21 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>429</v>
+        <v>437</v>
       </c>
       <c r="B24" t="s">
-        <v>430</v>
+        <v>438</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
       </c>
-      <c r="D24">
-        <v>2015</v>
-      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>140</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -2027,24 +2475,21 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>153</v>
+        <v>204</v>
       </c>
       <c r="B26" t="s">
-        <v>425</v>
+        <v>205</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
-      <c r="D26">
-        <v>2015</v>
-      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>153</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>372</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
@@ -2052,239 +2497,242 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>373</v>
+        <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>155</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>374</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>375</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>157</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>376</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="B32" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32">
-        <v>2015</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>422</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>424</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33">
-        <v>2015</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>370</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>371</v>
+        <v>47</v>
       </c>
       <c r="C34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34">
-        <v>2015</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>370</v>
+        <v>48</v>
       </c>
       <c r="B35" t="s">
-        <v>371</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>158</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>377</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>167</v>
+        <v>418</v>
       </c>
       <c r="B37" t="s">
-        <v>168</v>
+        <v>433</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
       </c>
+      <c r="D37">
+        <v>2015</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>169</v>
+        <v>420</v>
       </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>435</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
+      <c r="D38">
+        <v>2015</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>170</v>
+        <v>417</v>
       </c>
       <c r="B39" t="s">
-        <v>171</v>
+        <v>432</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
       </c>
+      <c r="D39">
+        <v>2015</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>172</v>
+        <v>419</v>
       </c>
       <c r="B40" t="s">
-        <v>173</v>
+        <v>434</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
       </c>
+      <c r="D40">
+        <v>2015</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>175</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>176</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>177</v>
+        <v>281</v>
       </c>
       <c r="B42" t="s">
-        <v>178</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>179</v>
+        <v>282</v>
       </c>
       <c r="B43" t="s">
-        <v>180</v>
+        <v>55</v>
       </c>
       <c r="C43" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>181</v>
+        <v>283</v>
       </c>
       <c r="B44" t="s">
-        <v>182</v>
+        <v>56</v>
       </c>
       <c r="C44" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>368</v>
+        <v>284</v>
       </c>
       <c r="B45" t="s">
-        <v>369</v>
+        <v>57</v>
       </c>
       <c r="C45" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>183</v>
+        <v>285</v>
       </c>
       <c r="B46" t="s">
-        <v>184</v>
+        <v>58</v>
       </c>
       <c r="C46" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>189</v>
+        <v>286</v>
       </c>
       <c r="B47" t="s">
-        <v>190</v>
+        <v>59</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>6</v>
+        <v>287</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="C48" t="s">
         <v>8</v>
@@ -2292,10 +2740,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>288</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="C49" t="s">
         <v>8</v>
@@ -2303,10 +2751,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>211</v>
+        <v>289</v>
       </c>
       <c r="B50" t="s">
-        <v>210</v>
+        <v>62</v>
       </c>
       <c r="C50" t="s">
         <v>8</v>
@@ -2314,10 +2762,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>290</v>
       </c>
       <c r="B51" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="C51" t="s">
         <v>8</v>
@@ -2325,10 +2773,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>21</v>
+        <v>291</v>
       </c>
       <c r="B52" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="C52" t="s">
         <v>8</v>
@@ -2336,10 +2784,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>42</v>
+        <v>292</v>
       </c>
       <c r="B53" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="C53" t="s">
         <v>8</v>
@@ -2347,10 +2795,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>409</v>
+        <v>293</v>
       </c>
       <c r="B54" t="s">
-        <v>410</v>
+        <v>66</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
@@ -2358,10 +2806,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>44</v>
+        <v>294</v>
       </c>
       <c r="B55" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="C55" t="s">
         <v>8</v>
@@ -2369,10 +2817,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>46</v>
+        <v>295</v>
       </c>
       <c r="B56" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="C56" t="s">
         <v>8</v>
@@ -2380,10 +2828,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>296</v>
       </c>
       <c r="B57" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="C57" t="s">
         <v>8</v>
@@ -2391,10 +2839,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>52</v>
+        <v>297</v>
       </c>
       <c r="B58" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="C58" t="s">
         <v>8</v>
@@ -2402,10 +2850,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
       <c r="B59" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C59" t="s">
         <v>8</v>
@@ -2413,10 +2861,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>282</v>
+        <v>299</v>
       </c>
       <c r="B60" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="C60" t="s">
         <v>8</v>
@@ -2424,10 +2872,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
       <c r="B61" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="C61" t="s">
         <v>8</v>
@@ -2435,10 +2883,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>284</v>
+        <v>301</v>
       </c>
       <c r="B62" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="C62" t="s">
         <v>8</v>
@@ -2446,10 +2894,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>285</v>
+        <v>302</v>
       </c>
       <c r="B63" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="C63" t="s">
         <v>8</v>
@@ -2457,10 +2905,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>286</v>
+        <v>303</v>
       </c>
       <c r="B64" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="C64" t="s">
         <v>8</v>
@@ -2468,10 +2916,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>287</v>
+        <v>304</v>
       </c>
       <c r="B65" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C65" t="s">
         <v>8</v>
@@ -2479,10 +2927,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>288</v>
+        <v>305</v>
       </c>
       <c r="B66" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="C66" t="s">
         <v>8</v>
@@ -2490,10 +2938,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>289</v>
+        <v>306</v>
       </c>
       <c r="B67" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="C67" t="s">
         <v>8</v>
@@ -2501,10 +2949,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>290</v>
+        <v>307</v>
       </c>
       <c r="B68" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C68" t="s">
         <v>8</v>
@@ -2512,10 +2960,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>291</v>
+        <v>308</v>
       </c>
       <c r="B69" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C69" t="s">
         <v>8</v>
@@ -2523,10 +2971,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>292</v>
+        <v>309</v>
       </c>
       <c r="B70" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="C70" t="s">
         <v>8</v>
@@ -2534,10 +2982,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>293</v>
+        <v>310</v>
       </c>
       <c r="B71" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C71" t="s">
         <v>8</v>
@@ -2545,10 +2993,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>294</v>
+        <v>311</v>
       </c>
       <c r="B72" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="C72" t="s">
         <v>8</v>
@@ -2556,10 +3004,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>295</v>
+        <v>312</v>
       </c>
       <c r="B73" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="C73" t="s">
         <v>8</v>
@@ -2567,10 +3015,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>296</v>
+        <v>313</v>
       </c>
       <c r="B74" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="C74" t="s">
         <v>8</v>
@@ -2578,10 +3026,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>297</v>
+        <v>314</v>
       </c>
       <c r="B75" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C75" t="s">
         <v>8</v>
@@ -2589,10 +3037,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>298</v>
+        <v>315</v>
       </c>
       <c r="B76" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="C76" t="s">
         <v>8</v>
@@ -2600,10 +3048,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>299</v>
+        <v>316</v>
       </c>
       <c r="B77" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C77" t="s">
         <v>8</v>
@@ -2611,10 +3059,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
       <c r="B78" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="C78" t="s">
         <v>8</v>
@@ -2622,10 +3070,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>301</v>
+        <v>318</v>
       </c>
       <c r="B79" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C79" t="s">
         <v>8</v>
@@ -2633,10 +3081,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>302</v>
+        <v>319</v>
       </c>
       <c r="B80" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="C80" t="s">
         <v>8</v>
@@ -2644,10 +3092,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>303</v>
+        <v>320</v>
       </c>
       <c r="B81" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="C81" t="s">
         <v>8</v>
@@ -2655,10 +3103,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>304</v>
+        <v>321</v>
       </c>
       <c r="B82" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="C82" t="s">
         <v>8</v>
@@ -2666,10 +3114,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
       <c r="B83" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="C83" t="s">
         <v>8</v>
@@ -2677,10 +3125,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>306</v>
+        <v>323</v>
       </c>
       <c r="B84" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="C84" t="s">
         <v>8</v>
@@ -2688,10 +3136,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>307</v>
+        <v>324</v>
       </c>
       <c r="B85" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="C85" t="s">
         <v>8</v>
@@ -2699,10 +3147,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>308</v>
+        <v>325</v>
       </c>
       <c r="B86" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="C86" t="s">
         <v>8</v>
@@ -2710,10 +3158,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>309</v>
+        <v>326</v>
       </c>
       <c r="B87" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="C87" t="s">
         <v>8</v>
@@ -2721,10 +3169,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>310</v>
+        <v>327</v>
       </c>
       <c r="B88" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="C88" t="s">
         <v>8</v>
@@ -2732,10 +3180,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>311</v>
+        <v>328</v>
       </c>
       <c r="B89" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="C89" t="s">
         <v>8</v>
@@ -2743,10 +3191,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>312</v>
+        <v>329</v>
       </c>
       <c r="B90" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="C90" t="s">
         <v>8</v>
@@ -2754,10 +3202,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>313</v>
+        <v>330</v>
       </c>
       <c r="B91" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C91" t="s">
         <v>8</v>
@@ -2765,10 +3213,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>314</v>
+        <v>331</v>
       </c>
       <c r="B92" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="C92" t="s">
         <v>8</v>
@@ -2776,10 +3224,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>315</v>
+        <v>332</v>
       </c>
       <c r="B93" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="C93" t="s">
         <v>8</v>
@@ -2787,10 +3235,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>316</v>
+        <v>333</v>
       </c>
       <c r="B94" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="C94" t="s">
         <v>8</v>
@@ -2798,10 +3246,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="B95" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="C95" t="s">
         <v>8</v>
@@ -2809,10 +3257,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>318</v>
+        <v>335</v>
       </c>
       <c r="B96" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="C96" t="s">
         <v>8</v>
@@ -2820,10 +3268,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>319</v>
+        <v>336</v>
       </c>
       <c r="B97" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="C97" t="s">
         <v>8</v>
@@ -2831,10 +3279,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>320</v>
+        <v>337</v>
       </c>
       <c r="B98" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C98" t="s">
         <v>8</v>
@@ -2842,10 +3290,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>321</v>
+        <v>338</v>
       </c>
       <c r="B99" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C99" t="s">
         <v>8</v>
@@ -2853,10 +3301,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>322</v>
+        <v>339</v>
       </c>
       <c r="B100" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="C100" t="s">
         <v>8</v>
@@ -2864,10 +3312,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>323</v>
+        <v>340</v>
       </c>
       <c r="B101" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="C101" t="s">
         <v>8</v>
@@ -2875,10 +3323,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>324</v>
+        <v>341</v>
       </c>
       <c r="B102" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="C102" t="s">
         <v>8</v>
@@ -2886,10 +3334,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>325</v>
+        <v>342</v>
       </c>
       <c r="B103" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="C103" t="s">
         <v>8</v>
@@ -2897,10 +3345,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>326</v>
+        <v>343</v>
       </c>
       <c r="B104" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="C104" t="s">
         <v>8</v>
@@ -2908,10 +3356,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>327</v>
+        <v>344</v>
       </c>
       <c r="B105" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="C105" t="s">
         <v>8</v>
@@ -2919,10 +3367,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>328</v>
+        <v>345</v>
       </c>
       <c r="B106" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="C106" t="s">
         <v>8</v>
@@ -2930,10 +3378,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>329</v>
+        <v>346</v>
       </c>
       <c r="B107" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="C107" t="s">
         <v>8</v>
@@ -2941,10 +3389,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>330</v>
+        <v>347</v>
       </c>
       <c r="B108" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="C108" t="s">
         <v>8</v>
@@ -2952,10 +3400,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>331</v>
+        <v>348</v>
       </c>
       <c r="B109" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="C109" t="s">
         <v>8</v>
@@ -2963,10 +3411,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>332</v>
+        <v>349</v>
       </c>
       <c r="B110" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="C110" t="s">
         <v>8</v>
@@ -2974,10 +3422,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>333</v>
+        <v>350</v>
       </c>
       <c r="B111" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="C111" t="s">
         <v>8</v>
@@ -2985,10 +3433,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>334</v>
+        <v>351</v>
       </c>
       <c r="B112" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="C112" t="s">
         <v>8</v>
@@ -2996,10 +3444,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>335</v>
+        <v>352</v>
       </c>
       <c r="B113" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C113" t="s">
         <v>8</v>
@@ -3007,10 +3455,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>336</v>
+        <v>353</v>
       </c>
       <c r="B114" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="C114" t="s">
         <v>8</v>
@@ -3018,10 +3466,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>337</v>
+        <v>354</v>
       </c>
       <c r="B115" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="C115" t="s">
         <v>8</v>
@@ -3029,10 +3477,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>338</v>
+        <v>355</v>
       </c>
       <c r="B116" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="C116" t="s">
         <v>8</v>
@@ -3040,10 +3488,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>339</v>
+        <v>356</v>
       </c>
       <c r="B117" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="C117" t="s">
         <v>8</v>
@@ -3051,10 +3499,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="B118" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="C118" t="s">
         <v>8</v>
@@ -3062,10 +3510,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>341</v>
+        <v>358</v>
       </c>
       <c r="B119" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="C119" t="s">
         <v>8</v>
@@ -3073,10 +3521,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>342</v>
+        <v>359</v>
       </c>
       <c r="B120" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="C120" t="s">
         <v>8</v>
@@ -3084,10 +3532,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>343</v>
+        <v>360</v>
       </c>
       <c r="B121" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="C121" t="s">
         <v>8</v>
@@ -3095,10 +3543,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>344</v>
+        <v>361</v>
       </c>
       <c r="B122" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="C122" t="s">
         <v>8</v>
@@ -3106,10 +3554,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>345</v>
+        <v>362</v>
       </c>
       <c r="B123" t="s">
-        <v>118</v>
+        <v>197</v>
       </c>
       <c r="C123" t="s">
         <v>8</v>
@@ -3117,10 +3565,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>346</v>
+        <v>363</v>
       </c>
       <c r="B124" t="s">
-        <v>119</v>
+        <v>200</v>
       </c>
       <c r="C124" t="s">
         <v>8</v>
@@ -3128,10 +3576,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>347</v>
+        <v>364</v>
       </c>
       <c r="B125" t="s">
-        <v>120</v>
+        <v>201</v>
       </c>
       <c r="C125" t="s">
         <v>8</v>
@@ -3139,10 +3587,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>348</v>
+        <v>365</v>
       </c>
       <c r="B126" t="s">
-        <v>121</v>
+        <v>202</v>
       </c>
       <c r="C126" t="s">
         <v>8</v>
@@ -3150,10 +3598,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>349</v>
+        <v>365</v>
       </c>
       <c r="B127" t="s">
-        <v>122</v>
+        <v>202</v>
       </c>
       <c r="C127" t="s">
         <v>8</v>
@@ -3161,10 +3609,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>350</v>
+        <v>215</v>
       </c>
       <c r="B128" t="s">
-        <v>123</v>
+        <v>259</v>
       </c>
       <c r="C128" t="s">
         <v>8</v>
@@ -3172,10 +3620,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>351</v>
+        <v>216</v>
       </c>
       <c r="B129" t="s">
-        <v>124</v>
+        <v>260</v>
       </c>
       <c r="C129" t="s">
         <v>8</v>
@@ -3183,10 +3631,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>352</v>
+        <v>217</v>
       </c>
       <c r="B130" t="s">
-        <v>125</v>
+        <v>261</v>
       </c>
       <c r="C130" t="s">
         <v>8</v>
@@ -3194,21 +3642,21 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>353</v>
+        <v>218</v>
       </c>
       <c r="B131" t="s">
-        <v>126</v>
+        <v>262</v>
       </c>
       <c r="C131" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>354</v>
+      <c r="A132" s="2" t="s">
+        <v>219</v>
       </c>
       <c r="B132" t="s">
-        <v>127</v>
+        <v>263</v>
       </c>
       <c r="C132" t="s">
         <v>8</v>
@@ -3216,54 +3664,54 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>355</v>
+        <v>220</v>
       </c>
       <c r="B133" t="s">
-        <v>128</v>
+        <v>264</v>
       </c>
       <c r="C133" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>356</v>
+      <c r="A134" s="2" t="s">
+        <v>221</v>
       </c>
       <c r="B134" t="s">
-        <v>129</v>
+        <v>265</v>
       </c>
       <c r="C134" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>357</v>
+      <c r="A135" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="B135" t="s">
-        <v>130</v>
+        <v>266</v>
       </c>
       <c r="C135" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>358</v>
+      <c r="A136" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="B136" t="s">
-        <v>131</v>
+        <v>267</v>
       </c>
       <c r="C136" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>359</v>
+      <c r="A137" s="3" t="s">
+        <v>224</v>
       </c>
       <c r="B137" t="s">
-        <v>132</v>
+        <v>268</v>
       </c>
       <c r="C137" t="s">
         <v>8</v>
@@ -3271,10 +3719,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>360</v>
+        <v>225</v>
       </c>
       <c r="B138" t="s">
-        <v>133</v>
+        <v>269</v>
       </c>
       <c r="C138" t="s">
         <v>8</v>
@@ -3282,10 +3730,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>361</v>
+        <v>226</v>
       </c>
       <c r="B139" t="s">
-        <v>134</v>
+        <v>270</v>
       </c>
       <c r="C139" t="s">
         <v>8</v>
@@ -3293,10 +3741,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>362</v>
+        <v>227</v>
       </c>
       <c r="B140" t="s">
-        <v>197</v>
+        <v>271</v>
       </c>
       <c r="C140" t="s">
         <v>8</v>
@@ -3304,10 +3752,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>363</v>
+        <v>228</v>
       </c>
       <c r="B141" t="s">
-        <v>200</v>
+        <v>272</v>
       </c>
       <c r="C141" t="s">
         <v>8</v>
@@ -3315,10 +3763,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>364</v>
+        <v>229</v>
       </c>
       <c r="B142" t="s">
-        <v>201</v>
+        <v>273</v>
       </c>
       <c r="C142" t="s">
         <v>8</v>
@@ -3326,10 +3774,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>365</v>
+        <v>230</v>
       </c>
       <c r="B143" t="s">
-        <v>202</v>
+        <v>274</v>
       </c>
       <c r="C143" t="s">
         <v>8</v>
@@ -3337,10 +3785,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>365</v>
+        <v>231</v>
       </c>
       <c r="B144" t="s">
-        <v>202</v>
+        <v>275</v>
       </c>
       <c r="C144" t="s">
         <v>8</v>
@@ -3348,10 +3796,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="B145" t="s">
-        <v>259</v>
+        <v>276</v>
       </c>
       <c r="C145" t="s">
         <v>8</v>
@@ -3359,10 +3807,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
       <c r="B146" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="C146" t="s">
         <v>8</v>
@@ -3370,10 +3818,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>217</v>
+        <v>234</v>
       </c>
       <c r="B147" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="C147" t="s">
         <v>8</v>
@@ -3381,21 +3829,21 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>218</v>
+        <v>235</v>
       </c>
       <c r="B148" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
       <c r="C148" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="2" t="s">
-        <v>219</v>
+      <c r="A149" t="s">
+        <v>236</v>
       </c>
       <c r="B149" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="C149" t="s">
         <v>8</v>
@@ -3403,54 +3851,54 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>220</v>
+        <v>237</v>
       </c>
       <c r="B150" t="s">
-        <v>264</v>
+        <v>238</v>
       </c>
       <c r="C150" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" s="2" t="s">
-        <v>221</v>
+      <c r="A151" t="s">
+        <v>239</v>
       </c>
       <c r="B151" t="s">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="C151" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="2" t="s">
-        <v>222</v>
+      <c r="A152" t="s">
+        <v>241</v>
       </c>
       <c r="B152" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
       <c r="C152" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="2" t="s">
-        <v>223</v>
+      <c r="A153" t="s">
+        <v>243</v>
       </c>
       <c r="B153" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="C153" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="3" t="s">
-        <v>224</v>
+      <c r="A154" t="s">
+        <v>245</v>
       </c>
       <c r="B154" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="C154" t="s">
         <v>8</v>
@@ -3458,10 +3906,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
       <c r="B155" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="C155" t="s">
         <v>8</v>
@@ -3469,10 +3917,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>226</v>
+        <v>249</v>
       </c>
       <c r="B156" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="C156" t="s">
         <v>8</v>
@@ -3480,10 +3928,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="B157" t="s">
-        <v>271</v>
+        <v>252</v>
       </c>
       <c r="C157" t="s">
         <v>8</v>
@@ -3491,10 +3939,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>228</v>
+        <v>253</v>
       </c>
       <c r="B158" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="C158" t="s">
         <v>8</v>
@@ -3502,10 +3950,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>229</v>
+        <v>255</v>
       </c>
       <c r="B159" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="C159" t="s">
         <v>8</v>
@@ -3513,10 +3961,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="B160" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="C160" t="s">
         <v>8</v>
@@ -3524,10 +3972,10 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>231</v>
+        <v>366</v>
       </c>
       <c r="B161" t="s">
-        <v>275</v>
+        <v>367</v>
       </c>
       <c r="C161" t="s">
         <v>8</v>
@@ -3535,10 +3983,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>232</v>
+        <v>383</v>
       </c>
       <c r="B162" t="s">
-        <v>276</v>
+        <v>384</v>
       </c>
       <c r="C162" t="s">
         <v>8</v>
@@ -3546,10 +3994,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>233</v>
+        <v>385</v>
       </c>
       <c r="B163" t="s">
-        <v>277</v>
+        <v>386</v>
       </c>
       <c r="C163" t="s">
         <v>8</v>
@@ -3557,10 +4005,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>234</v>
+        <v>387</v>
       </c>
       <c r="B164" t="s">
-        <v>278</v>
+        <v>388</v>
       </c>
       <c r="C164" t="s">
         <v>8</v>
@@ -3568,10 +4016,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>235</v>
+        <v>389</v>
       </c>
       <c r="B165" t="s">
-        <v>279</v>
+        <v>390</v>
       </c>
       <c r="C165" t="s">
         <v>8</v>
@@ -3579,10 +4027,10 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>236</v>
+        <v>391</v>
       </c>
       <c r="B166" t="s">
-        <v>280</v>
+        <v>392</v>
       </c>
       <c r="C166" t="s">
         <v>8</v>
@@ -3590,10 +4038,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>237</v>
+        <v>395</v>
       </c>
       <c r="B167" t="s">
-        <v>238</v>
+        <v>396</v>
       </c>
       <c r="C167" t="s">
         <v>8</v>
@@ -3601,10 +4049,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>239</v>
+        <v>397</v>
       </c>
       <c r="B168" t="s">
-        <v>240</v>
+        <v>398</v>
       </c>
       <c r="C168" t="s">
         <v>8</v>
@@ -3612,10 +4060,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>241</v>
+        <v>399</v>
       </c>
       <c r="B169" t="s">
-        <v>242</v>
+        <v>400</v>
       </c>
       <c r="C169" t="s">
         <v>8</v>
@@ -3623,10 +4071,10 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>243</v>
+        <v>401</v>
       </c>
       <c r="B170" t="s">
-        <v>244</v>
+        <v>402</v>
       </c>
       <c r="C170" t="s">
         <v>8</v>
@@ -3634,10 +4082,10 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>245</v>
+        <v>403</v>
       </c>
       <c r="B171" t="s">
-        <v>246</v>
+        <v>404</v>
       </c>
       <c r="C171" t="s">
         <v>8</v>
@@ -3645,10 +4093,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>247</v>
+        <v>405</v>
       </c>
       <c r="B172" t="s">
-        <v>248</v>
+        <v>406</v>
       </c>
       <c r="C172" t="s">
         <v>8</v>
@@ -3656,10 +4104,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>249</v>
+        <v>408</v>
       </c>
       <c r="B173" t="s">
-        <v>250</v>
+        <v>407</v>
       </c>
       <c r="C173" t="s">
         <v>8</v>
@@ -3667,10 +4115,10 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>251</v>
+        <v>443</v>
       </c>
       <c r="B174" t="s">
-        <v>252</v>
+        <v>444</v>
       </c>
       <c r="C174" t="s">
         <v>8</v>
@@ -3678,10 +4126,10 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>253</v>
+        <v>445</v>
       </c>
       <c r="B175" t="s">
-        <v>254</v>
+        <v>446</v>
       </c>
       <c r="C175" t="s">
         <v>8</v>
@@ -3689,10 +4137,10 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>255</v>
+        <v>447</v>
       </c>
       <c r="B176" t="s">
-        <v>256</v>
+        <v>448</v>
       </c>
       <c r="C176" t="s">
         <v>8</v>
@@ -3700,10 +4148,10 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>257</v>
+        <v>449</v>
       </c>
       <c r="B177" t="s">
-        <v>258</v>
+        <v>450</v>
       </c>
       <c r="C177" t="s">
         <v>8</v>
@@ -3711,10 +4159,10 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>366</v>
+        <v>451</v>
       </c>
       <c r="B178" t="s">
-        <v>367</v>
+        <v>452</v>
       </c>
       <c r="C178" t="s">
         <v>8</v>
@@ -3722,10 +4170,10 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>383</v>
+        <v>453</v>
       </c>
       <c r="B179" t="s">
-        <v>384</v>
+        <v>454</v>
       </c>
       <c r="C179" t="s">
         <v>8</v>
@@ -3733,10 +4181,10 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>385</v>
+        <v>455</v>
       </c>
       <c r="B180" t="s">
-        <v>386</v>
+        <v>456</v>
       </c>
       <c r="C180" t="s">
         <v>8</v>
@@ -3744,10 +4192,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>387</v>
+        <v>457</v>
       </c>
       <c r="B181" t="s">
-        <v>388</v>
+        <v>458</v>
       </c>
       <c r="C181" t="s">
         <v>8</v>
@@ -3755,10 +4203,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>389</v>
+        <v>459</v>
       </c>
       <c r="B182" t="s">
-        <v>390</v>
+        <v>460</v>
       </c>
       <c r="C182" t="s">
         <v>8</v>
@@ -3766,10 +4214,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>391</v>
+        <v>461</v>
       </c>
       <c r="B183" t="s">
-        <v>392</v>
+        <v>462</v>
       </c>
       <c r="C183" t="s">
         <v>8</v>
@@ -3777,10 +4225,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>395</v>
+        <v>463</v>
       </c>
       <c r="B184" t="s">
-        <v>396</v>
+        <v>464</v>
       </c>
       <c r="C184" t="s">
         <v>8</v>
@@ -3788,10 +4236,10 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>397</v>
+        <v>465</v>
       </c>
       <c r="B185" t="s">
-        <v>398</v>
+        <v>466</v>
       </c>
       <c r="C185" t="s">
         <v>8</v>
@@ -3799,10 +4247,10 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>399</v>
+        <v>467</v>
       </c>
       <c r="B186" t="s">
-        <v>400</v>
+        <v>468</v>
       </c>
       <c r="C186" t="s">
         <v>8</v>
@@ -3810,10 +4258,10 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>401</v>
+        <v>469</v>
       </c>
       <c r="B187" t="s">
-        <v>402</v>
+        <v>470</v>
       </c>
       <c r="C187" t="s">
         <v>8</v>
@@ -3821,10 +4269,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>403</v>
+        <v>471</v>
       </c>
       <c r="B188" t="s">
-        <v>404</v>
+        <v>472</v>
       </c>
       <c r="C188" t="s">
         <v>8</v>
@@ -3832,10 +4280,10 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>405</v>
+        <v>473</v>
       </c>
       <c r="B189" t="s">
-        <v>406</v>
+        <v>474</v>
       </c>
       <c r="C189" t="s">
         <v>8</v>
@@ -3843,10 +4291,10 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>408</v>
+        <v>475</v>
       </c>
       <c r="B190" t="s">
-        <v>407</v>
+        <v>476</v>
       </c>
       <c r="C190" t="s">
         <v>8</v>
@@ -3854,10 +4302,10 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>135</v>
+        <v>477</v>
       </c>
       <c r="B191" t="s">
-        <v>136</v>
+        <v>478</v>
       </c>
       <c r="C191" t="s">
         <v>8</v>
@@ -3865,10 +4313,10 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>141</v>
+        <v>479</v>
       </c>
       <c r="B192" t="s">
-        <v>142</v>
+        <v>480</v>
       </c>
       <c r="C192" t="s">
         <v>8</v>
@@ -3876,10 +4324,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>143</v>
+        <v>481</v>
       </c>
       <c r="B193" t="s">
-        <v>144</v>
+        <v>482</v>
       </c>
       <c r="C193" t="s">
         <v>8</v>
@@ -3887,10 +4335,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>185</v>
+        <v>483</v>
       </c>
       <c r="B194" t="s">
-        <v>186</v>
+        <v>484</v>
       </c>
       <c r="C194" t="s">
         <v>8</v>
@@ -3898,350 +4346,1231 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>393</v>
+        <v>485</v>
       </c>
       <c r="B195" t="s">
-        <v>394</v>
+        <v>486</v>
       </c>
       <c r="C195" t="s">
-        <v>214</v>
+        <v>8</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>212</v>
+        <v>487</v>
       </c>
       <c r="B196" t="s">
-        <v>213</v>
+        <v>488</v>
       </c>
       <c r="C196" t="s">
-        <v>214</v>
+        <v>8</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>23</v>
+        <v>489</v>
       </c>
       <c r="B197" t="s">
-        <v>24</v>
+        <v>490</v>
       </c>
       <c r="C197" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>26</v>
+        <v>491</v>
       </c>
       <c r="B198" t="s">
-        <v>27</v>
+        <v>492</v>
       </c>
       <c r="C198" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>28</v>
+        <v>493</v>
       </c>
       <c r="B199" t="s">
-        <v>29</v>
+        <v>494</v>
       </c>
       <c r="C199" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>30</v>
+        <v>495</v>
       </c>
       <c r="B200" t="s">
-        <v>31</v>
+        <v>496</v>
       </c>
       <c r="C200" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>38</v>
+        <v>497</v>
       </c>
       <c r="B201" t="s">
-        <v>39</v>
+        <v>498</v>
       </c>
       <c r="C201" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>40</v>
+        <v>499</v>
       </c>
       <c r="B202" t="s">
-        <v>41</v>
+        <v>500</v>
       </c>
       <c r="C202" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>50</v>
+        <v>501</v>
       </c>
       <c r="B203" t="s">
-        <v>51</v>
+        <v>502</v>
       </c>
       <c r="C203" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>137</v>
+        <v>503</v>
       </c>
       <c r="B204" t="s">
-        <v>138</v>
+        <v>504</v>
       </c>
       <c r="C204" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>145</v>
+        <v>505</v>
       </c>
       <c r="B205" t="s">
-        <v>146</v>
+        <v>506</v>
       </c>
       <c r="C205" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>147</v>
+        <v>507</v>
       </c>
       <c r="B206" t="s">
-        <v>148</v>
+        <v>508</v>
       </c>
       <c r="C206" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>149</v>
+        <v>509</v>
       </c>
       <c r="B207" t="s">
-        <v>150</v>
+        <v>510</v>
       </c>
       <c r="C207" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>151</v>
+        <v>511</v>
       </c>
       <c r="B208" t="s">
-        <v>152</v>
+        <v>512</v>
       </c>
       <c r="C208" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>159</v>
+        <v>513</v>
       </c>
       <c r="B209" t="s">
-        <v>160</v>
+        <v>514</v>
       </c>
       <c r="C209" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>161</v>
+        <v>515</v>
       </c>
       <c r="B210" t="s">
-        <v>162</v>
+        <v>516</v>
       </c>
       <c r="C210" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>163</v>
+        <v>517</v>
       </c>
       <c r="B211" t="s">
-        <v>164</v>
+        <v>518</v>
       </c>
       <c r="C211" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>165</v>
+        <v>519</v>
       </c>
       <c r="B212" t="s">
-        <v>166</v>
+        <v>520</v>
       </c>
       <c r="C212" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>208</v>
+        <v>521</v>
       </c>
       <c r="B213" t="s">
-        <v>209</v>
+        <v>522</v>
       </c>
       <c r="C213" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>187</v>
+        <v>523</v>
       </c>
       <c r="B214" t="s">
-        <v>188</v>
+        <v>524</v>
       </c>
       <c r="C214" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>191</v>
+        <v>525</v>
       </c>
       <c r="B215" t="s">
-        <v>192</v>
+        <v>526</v>
       </c>
       <c r="C215" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>193</v>
+        <v>527</v>
       </c>
       <c r="B216" t="s">
-        <v>194</v>
+        <v>528</v>
       </c>
       <c r="C216" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>195</v>
+        <v>529</v>
       </c>
       <c r="B217" t="s">
-        <v>196</v>
+        <v>530</v>
       </c>
       <c r="C217" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>11</v>
+        <v>531</v>
       </c>
       <c r="B218" t="s">
-        <v>12</v>
+        <v>532</v>
       </c>
       <c r="C218" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>15</v>
+        <v>533</v>
       </c>
       <c r="B219" t="s">
-        <v>16</v>
+        <v>534</v>
       </c>
       <c r="C219" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>198</v>
+        <v>535</v>
       </c>
       <c r="B220" t="s">
-        <v>199</v>
+        <v>536</v>
       </c>
       <c r="C220" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
+        <v>537</v>
+      </c>
+      <c r="B221" t="s">
+        <v>538</v>
+      </c>
+      <c r="C221" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="B222" t="s">
+        <v>540</v>
+      </c>
+      <c r="C222" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="B223" t="s">
+        <v>542</v>
+      </c>
+      <c r="C223" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="B224" t="s">
+        <v>544</v>
+      </c>
+      <c r="C224" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="B225" t="s">
+        <v>546</v>
+      </c>
+      <c r="C225" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="B226" t="s">
+        <v>548</v>
+      </c>
+      <c r="C226" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="B227" t="s">
+        <v>550</v>
+      </c>
+      <c r="C227" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="B228" t="s">
+        <v>552</v>
+      </c>
+      <c r="C228" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="B229" t="s">
+        <v>554</v>
+      </c>
+      <c r="C229" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="B230" t="s">
+        <v>556</v>
+      </c>
+      <c r="C230" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="B231" t="s">
+        <v>558</v>
+      </c>
+      <c r="C231" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="B232" t="s">
+        <v>560</v>
+      </c>
+      <c r="C232" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="B233" t="s">
+        <v>562</v>
+      </c>
+      <c r="C233" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="B234" t="s">
+        <v>564</v>
+      </c>
+      <c r="C234" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="B235" t="s">
+        <v>566</v>
+      </c>
+      <c r="C235" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="B236" t="s">
+        <v>568</v>
+      </c>
+      <c r="C236" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="B237" t="s">
+        <v>570</v>
+      </c>
+      <c r="C237" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B238" t="s">
+        <v>572</v>
+      </c>
+      <c r="C238" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="B239" t="s">
+        <v>574</v>
+      </c>
+      <c r="C239" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="B240" t="s">
+        <v>576</v>
+      </c>
+      <c r="C240" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="B241" t="s">
+        <v>578</v>
+      </c>
+      <c r="C241" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="B242" t="s">
+        <v>580</v>
+      </c>
+      <c r="C242" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="B243" t="s">
+        <v>582</v>
+      </c>
+      <c r="C243" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="B244" t="s">
+        <v>586</v>
+      </c>
+      <c r="C244" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="B245" t="s">
+        <v>588</v>
+      </c>
+      <c r="C245" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="B246" t="s">
+        <v>590</v>
+      </c>
+      <c r="C246" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="B247" t="s">
+        <v>592</v>
+      </c>
+      <c r="C247" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="B248" t="s">
+        <v>594</v>
+      </c>
+      <c r="C248" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="B249" t="s">
+        <v>596</v>
+      </c>
+      <c r="C249" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>393</v>
+      </c>
+      <c r="B250" t="s">
+        <v>394</v>
+      </c>
+      <c r="C250" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>135</v>
+      </c>
+      <c r="B251" t="s">
+        <v>136</v>
+      </c>
+      <c r="C251" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>411</v>
+      </c>
+      <c r="B252" t="s">
+        <v>412</v>
+      </c>
+      <c r="C252" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>415</v>
+      </c>
+      <c r="B253" t="s">
+        <v>428</v>
+      </c>
+      <c r="C253" t="s">
+        <v>5</v>
+      </c>
+      <c r="D253">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>137</v>
+      </c>
+      <c r="B254" t="s">
+        <v>138</v>
+      </c>
+      <c r="C254" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>413</v>
+      </c>
+      <c r="B255" t="s">
+        <v>426</v>
+      </c>
+      <c r="C255" t="s">
+        <v>5</v>
+      </c>
+      <c r="D255">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>414</v>
+      </c>
+      <c r="B256" t="s">
+        <v>427</v>
+      </c>
+      <c r="C256" t="s">
+        <v>5</v>
+      </c>
+      <c r="D256">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>429</v>
+      </c>
+      <c r="B257" t="s">
+        <v>430</v>
+      </c>
+      <c r="C257" t="s">
+        <v>5</v>
+      </c>
+      <c r="D257">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>139</v>
+      </c>
+      <c r="B258" t="s">
+        <v>140</v>
+      </c>
+      <c r="C258" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>141</v>
+      </c>
+      <c r="B259" t="s">
+        <v>142</v>
+      </c>
+      <c r="C259" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>378</v>
+      </c>
+      <c r="B260" t="s">
+        <v>379</v>
+      </c>
+      <c r="C260" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>143</v>
+      </c>
+      <c r="B261" t="s">
+        <v>144</v>
+      </c>
+      <c r="C261" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>198</v>
+      </c>
+      <c r="B262" t="s">
+        <v>199</v>
+      </c>
+      <c r="C262" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>145</v>
+      </c>
+      <c r="B263" t="s">
+        <v>146</v>
+      </c>
+      <c r="C263" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>147</v>
+      </c>
+      <c r="B264" t="s">
+        <v>148</v>
+      </c>
+      <c r="C264" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>149</v>
+      </c>
+      <c r="B265" t="s">
+        <v>150</v>
+      </c>
+      <c r="C265" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>151</v>
+      </c>
+      <c r="B266" t="s">
+        <v>152</v>
+      </c>
+      <c r="C266" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>153</v>
+      </c>
+      <c r="B267" t="s">
+        <v>425</v>
+      </c>
+      <c r="C267" t="s">
+        <v>5</v>
+      </c>
+      <c r="D267">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>153</v>
+      </c>
+      <c r="B268" t="s">
+        <v>372</v>
+      </c>
+      <c r="C268" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>154</v>
+      </c>
+      <c r="B269" t="s">
+        <v>373</v>
+      </c>
+      <c r="C269" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>155</v>
+      </c>
+      <c r="B270" t="s">
+        <v>374</v>
+      </c>
+      <c r="C270" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>156</v>
+      </c>
+      <c r="B271" t="s">
+        <v>375</v>
+      </c>
+      <c r="C271" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>157</v>
+      </c>
+      <c r="B272" t="s">
+        <v>376</v>
+      </c>
+      <c r="C272" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>421</v>
+      </c>
+      <c r="B273" t="s">
+        <v>423</v>
+      </c>
+      <c r="C273" t="s">
+        <v>5</v>
+      </c>
+      <c r="D273">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>422</v>
+      </c>
+      <c r="B274" t="s">
+        <v>424</v>
+      </c>
+      <c r="C274" t="s">
+        <v>5</v>
+      </c>
+      <c r="D274">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>370</v>
+      </c>
+      <c r="B275" t="s">
+        <v>371</v>
+      </c>
+      <c r="C275" t="s">
+        <v>5</v>
+      </c>
+      <c r="D275">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>370</v>
+      </c>
+      <c r="B276" t="s">
+        <v>371</v>
+      </c>
+      <c r="C276" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>158</v>
+      </c>
+      <c r="B277" t="s">
+        <v>377</v>
+      </c>
+      <c r="C277" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>159</v>
+      </c>
+      <c r="B278" t="s">
+        <v>160</v>
+      </c>
+      <c r="C278" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>161</v>
+      </c>
+      <c r="B279" t="s">
+        <v>162</v>
+      </c>
+      <c r="C279" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
         <v>206</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B280" t="s">
         <v>207</v>
       </c>
-      <c r="C221" t="s">
+      <c r="C280" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>163</v>
+      </c>
+      <c r="B281" t="s">
+        <v>164</v>
+      </c>
+      <c r="C281" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>165</v>
+      </c>
+      <c r="B282" t="s">
+        <v>166</v>
+      </c>
+      <c r="C282" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>167</v>
+      </c>
+      <c r="B283" t="s">
+        <v>168</v>
+      </c>
+      <c r="C283" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>169</v>
+      </c>
+      <c r="B284" t="s">
+        <v>20</v>
+      </c>
+      <c r="C284" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>170</v>
+      </c>
+      <c r="B285" t="s">
+        <v>171</v>
+      </c>
+      <c r="C285" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>172</v>
+      </c>
+      <c r="B286" t="s">
+        <v>173</v>
+      </c>
+      <c r="C286" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
         <v>174</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B287" t="s">
         <v>37</v>
       </c>
-      <c r="C222" t="s">
+      <c r="C287" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
-        <v>11</v>
-      </c>
-      <c r="B223" t="s">
-        <v>12</v>
-      </c>
-      <c r="C223" t="s">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>175</v>
+      </c>
+      <c r="B288" t="s">
+        <v>176</v>
+      </c>
+      <c r="C288" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>177</v>
+      </c>
+      <c r="B289" t="s">
+        <v>178</v>
+      </c>
+      <c r="C289" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>179</v>
+      </c>
+      <c r="B290" t="s">
+        <v>180</v>
+      </c>
+      <c r="C290" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>181</v>
+      </c>
+      <c r="B291" t="s">
+        <v>182</v>
+      </c>
+      <c r="C291" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>368</v>
+      </c>
+      <c r="B292" t="s">
+        <v>369</v>
+      </c>
+      <c r="C292" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>183</v>
+      </c>
+      <c r="B293" t="s">
+        <v>184</v>
+      </c>
+      <c r="C293" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>208</v>
+      </c>
+      <c r="B294" t="s">
+        <v>209</v>
+      </c>
+      <c r="C294" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>185</v>
+      </c>
+      <c r="B295" t="s">
+        <v>186</v>
+      </c>
+      <c r="C295" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>212</v>
+      </c>
+      <c r="B296" t="s">
+        <v>213</v>
+      </c>
+      <c r="C296" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>187</v>
+      </c>
+      <c r="B297" t="s">
+        <v>188</v>
+      </c>
+      <c r="C297" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>189</v>
+      </c>
+      <c r="B298" t="s">
+        <v>190</v>
+      </c>
+      <c r="C298" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>583</v>
+      </c>
+      <c r="B299" t="s">
+        <v>584</v>
+      </c>
+      <c r="C299" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>441</v>
+      </c>
+      <c r="B300" t="s">
+        <v>442</v>
+      </c>
+      <c r="C300" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
-        <v>15</v>
-      </c>
-      <c r="B224" t="s">
-        <v>16</v>
-      </c>
-      <c r="C224" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
-        <v>378</v>
-      </c>
-      <c r="B225" t="s">
-        <v>379</v>
-      </c>
-      <c r="C225" t="s">
-        <v>380</v>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>191</v>
+      </c>
+      <c r="B301" t="s">
+        <v>192</v>
+      </c>
+      <c r="C301" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>193</v>
+      </c>
+      <c r="B302" t="s">
+        <v>194</v>
+      </c>
+      <c r="C302" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>195</v>
+      </c>
+      <c r="B303" t="s">
+        <v>196</v>
+      </c>
+      <c r="C303" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D225">
-    <sortCondition ref="C2:C225"/>
-    <sortCondition ref="A2:A225"/>
-    <sortCondition ref="D2:D225"/>
+  <sortState ref="A2:E303">
+    <sortCondition ref="A2:A303"/>
+    <sortCondition ref="D2:D303"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>